<commit_message>
add integration test with registration and leave feature
</commit_message>
<xml_diff>
--- a/Documents/1_TestCases/TC04_Integration/TC04_Integration_TestCase.xlsx
+++ b/Documents/1_TestCases/TC04_Integration/TC04_Integration_TestCase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java\Automation\OrangeHRM---Automation-Java-Playwright-JUnit-\Documents\1_TestCases\TC04_Integration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05730429-4014-41B2-B6DB-4E5FCBB67500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35A53B7F-CEF3-4E84-BBF4-656916BCD607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="2115" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin" sheetId="1" r:id="rId1"/>
@@ -956,7 +956,7 @@
   <dimension ref="B2:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>